<commit_message>
fixes in w-method statistics
</commit_message>
<xml_diff>
--- a/py/tests/new_struct_sim_experiments/2_symbols/results/inter_n/n_fisso_10/results_2_symbols_n_10.xlsx
+++ b/py/tests/new_struct_sim_experiments/2_symbols/results/inter_n/n_fisso_10/results_2_symbols_n_10.xlsx
@@ -15018,7 +15018,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -15342,17 +15354,88 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1025076880"/>
-        <c:axId val="-1024969152"/>
+        <c:axId val="-761194512"/>
+        <c:axId val="-841894592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1025076880"/>
+        <c:axId val="-761194512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -15390,7 +15473,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1024969152"/>
+        <c:crossAx val="-841894592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15398,7 +15481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1024969152"/>
+        <c:axId val="-841894592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15418,6 +15501,63 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Average similarity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -15448,7 +15588,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1025076880"/>
+        <c:crossAx val="-761194512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15460,6 +15600,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -15572,7 +15744,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -15896,17 +16080,88 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1185195120"/>
-        <c:axId val="-1184969792"/>
+        <c:axId val="-760665104"/>
+        <c:axId val="-760607168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1185195120"/>
+        <c:axId val="-760665104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -15944,7 +16199,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1184969792"/>
+        <c:crossAx val="-760607168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15952,7 +16207,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1184969792"/>
+        <c:axId val="-760607168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15972,6 +16227,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Variance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -16002,7 +16313,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1185195120"/>
+        <c:crossAx val="-760665104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16014,6 +16325,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -16066,6 +16409,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Iterations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -16126,7 +16494,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -16450,17 +16830,88 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1077301376"/>
-        <c:axId val="-1075011920"/>
+        <c:axId val="-841075568"/>
+        <c:axId val="-841073248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1077301376"/>
+        <c:axId val="-841075568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -16498,7 +16949,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1075011920"/>
+        <c:crossAx val="-841073248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16506,7 +16957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1075011920"/>
+        <c:axId val="-841073248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16526,6 +16977,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Average iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -16556,7 +17063,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1077301376"/>
+        <c:crossAx val="-841075568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16568,6 +17075,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -16658,7 +17197,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -16766,11 +17305,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -16781,11 +17315,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -16817,9 +17346,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -17174,7 +17700,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -17282,11 +17808,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -17297,11 +17818,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -17333,9 +17849,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -17690,7 +18203,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -17798,11 +18311,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -17813,11 +18321,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -17849,9 +18352,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -18209,14 +18709,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>110</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>135</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -18239,16 +18739,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>136</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>159</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18270,13 +18770,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
+      <xdr:colOff>660400</xdr:colOff>
       <xdr:row>110</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>135</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -18589,7 +19089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:KF159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H108" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M100" workbookViewId="0">
       <selection activeCell="D110" activeCellId="1" sqref="A110:A159 D110:D159"/>
     </sheetView>
   </sheetViews>

</xml_diff>